<commit_message>
Updated Total Launch Times
</commit_message>
<xml_diff>
--- a/SensitivityAnalysisSpreadSheets/Holdback Bar Time/HoldbackBarTime10 Aircraft 9_1_+10%.xlsx
+++ b/SensitivityAnalysisSpreadSheets/Holdback Bar Time/HoldbackBarTime10 Aircraft 9_1_+10%.xlsx
@@ -79895,6 +79895,9 @@
           <t>Run 1</t>
         </is>
       </c>
+      <c r="B2" t="n">
+        <v>12.88716666666667</v>
+      </c>
       <c r="C2" t="n">
         <v>439.6822222222222</v>
       </c>
@@ -79950,6 +79953,9 @@
           <t>Run 2</t>
         </is>
       </c>
+      <c r="B3" t="n">
+        <v>13.95566666666667</v>
+      </c>
       <c r="C3" t="n">
         <v>445.0183333333333</v>
       </c>
@@ -80005,6 +80011,9 @@
           <t>Run 3</t>
         </is>
       </c>
+      <c r="B4" t="n">
+        <v>12.943</v>
+      </c>
       <c r="C4" t="n">
         <v>436.7872222222222</v>
       </c>
@@ -80060,6 +80069,9 @@
           <t>Run 4</t>
         </is>
       </c>
+      <c r="B5" t="n">
+        <v>14.942</v>
+      </c>
       <c r="C5" t="n">
         <v>445.7727777777778</v>
       </c>
@@ -80115,6 +80127,9 @@
           <t>Run 5</t>
         </is>
       </c>
+      <c r="B6" t="n">
+        <v>12.50816666666667</v>
+      </c>
       <c r="C6" t="n">
         <v>448.1261111111111</v>
       </c>
@@ -80170,6 +80185,9 @@
           <t>Run 6</t>
         </is>
       </c>
+      <c r="B7" t="n">
+        <v>13.1685</v>
+      </c>
       <c r="C7" t="n">
         <v>451.7950000000001</v>
       </c>
@@ -80225,6 +80243,9 @@
           <t>Run 7</t>
         </is>
       </c>
+      <c r="B8" t="n">
+        <v>14.52933333333333</v>
+      </c>
       <c r="C8" t="n">
         <v>469.5516666666667</v>
       </c>
@@ -80280,6 +80301,9 @@
           <t>Run 8</t>
         </is>
       </c>
+      <c r="B9" t="n">
+        <v>13.12666666666667</v>
+      </c>
       <c r="C9" t="n">
         <v>463.1588888888889</v>
       </c>
@@ -80335,6 +80359,9 @@
           <t>Run 9</t>
         </is>
       </c>
+      <c r="B10" t="n">
+        <v>13.65266666666667</v>
+      </c>
       <c r="C10" t="n">
         <v>447.6011111111111</v>
       </c>
@@ -80390,6 +80417,9 @@
           <t>Run 10</t>
         </is>
       </c>
+      <c r="B11" t="n">
+        <v>12.22483333333333</v>
+      </c>
       <c r="C11" t="n">
         <v>409.78</v>
       </c>
@@ -80445,6 +80475,9 @@
           <t>Run 11</t>
         </is>
       </c>
+      <c r="B12" t="n">
+        <v>12.80166666666667</v>
+      </c>
       <c r="C12" t="n">
         <v>423.8105555555556</v>
       </c>
@@ -80500,6 +80533,9 @@
           <t>Run 12</t>
         </is>
       </c>
+      <c r="B13" t="n">
+        <v>12.0065</v>
+      </c>
       <c r="C13" t="n">
         <v>423.6922222222222</v>
       </c>
@@ -80555,6 +80591,9 @@
           <t>Run 13</t>
         </is>
       </c>
+      <c r="B14" t="n">
+        <v>13.30066666666667</v>
+      </c>
       <c r="C14" t="n">
         <v>446.6583333333334</v>
       </c>
@@ -80610,6 +80649,9 @@
           <t>Run 14</t>
         </is>
       </c>
+      <c r="B15" t="n">
+        <v>13.0155</v>
+      </c>
       <c r="C15" t="n">
         <v>453.7038888888889</v>
       </c>
@@ -80665,6 +80707,9 @@
           <t>Run 15</t>
         </is>
       </c>
+      <c r="B16" t="n">
+        <v>13.31333333333333</v>
+      </c>
       <c r="C16" t="n">
         <v>442.0077777777778</v>
       </c>
@@ -80720,6 +80765,9 @@
           <t>Run 16</t>
         </is>
       </c>
+      <c r="B17" t="n">
+        <v>14.53566666666667</v>
+      </c>
       <c r="C17" t="n">
         <v>444.7233333333334</v>
       </c>
@@ -80775,6 +80823,9 @@
           <t>Run 17</t>
         </is>
       </c>
+      <c r="B18" t="n">
+        <v>12.306</v>
+      </c>
       <c r="C18" t="n">
         <v>442.7766666666666</v>
       </c>
@@ -80830,6 +80881,9 @@
           <t>Run 18</t>
         </is>
       </c>
+      <c r="B19" t="n">
+        <v>13.00983333333333</v>
+      </c>
       <c r="C19" t="n">
         <v>440.2622222222222</v>
       </c>
@@ -80885,6 +80939,9 @@
           <t>Run 19</t>
         </is>
       </c>
+      <c r="B20" t="n">
+        <v>12.84166666666667</v>
+      </c>
       <c r="C20" t="n">
         <v>433.0655555555555</v>
       </c>
@@ -80940,6 +80997,9 @@
           <t>Run 20</t>
         </is>
       </c>
+      <c r="B21" t="n">
+        <v>14.42633333333333</v>
+      </c>
       <c r="C21" t="n">
         <v>447.6044444444444</v>
       </c>
@@ -80995,6 +81055,9 @@
           <t>Run 21</t>
         </is>
       </c>
+      <c r="B22" t="n">
+        <v>15.027</v>
+      </c>
       <c r="C22" t="n">
         <v>452.2111111111111</v>
       </c>
@@ -81050,6 +81113,9 @@
           <t>Run 22</t>
         </is>
       </c>
+      <c r="B23" t="n">
+        <v>13.3795</v>
+      </c>
       <c r="C23" t="n">
         <v>458.61</v>
       </c>
@@ -81105,6 +81171,9 @@
           <t>Run 23</t>
         </is>
       </c>
+      <c r="B24" t="n">
+        <v>13.78383333333333</v>
+      </c>
       <c r="C24" t="n">
         <v>451.0916666666667</v>
       </c>
@@ -81160,6 +81229,9 @@
           <t>Run 24</t>
         </is>
       </c>
+      <c r="B25" t="n">
+        <v>12.128</v>
+      </c>
       <c r="C25" t="n">
         <v>414.453888888889</v>
       </c>
@@ -81215,6 +81287,9 @@
           <t>Run 25</t>
         </is>
       </c>
+      <c r="B26" t="n">
+        <v>13.959</v>
+      </c>
       <c r="C26" t="n">
         <v>450.7522222222223</v>
       </c>
@@ -81270,6 +81345,9 @@
           <t>Run 26</t>
         </is>
       </c>
+      <c r="B27" t="n">
+        <v>12.5815</v>
+      </c>
       <c r="C27" t="n">
         <v>431.5911111111111</v>
       </c>
@@ -81325,6 +81403,9 @@
           <t>Run 27</t>
         </is>
       </c>
+      <c r="B28" t="n">
+        <v>13.81133333333333</v>
+      </c>
       <c r="C28" t="n">
         <v>440.13</v>
       </c>
@@ -81380,6 +81461,9 @@
           <t>Run 28</t>
         </is>
       </c>
+      <c r="B29" t="n">
+        <v>14.01</v>
+      </c>
       <c r="C29" t="n">
         <v>455.705</v>
       </c>
@@ -81435,6 +81519,9 @@
           <t>Run 29</t>
         </is>
       </c>
+      <c r="B30" t="n">
+        <v>14.1885</v>
+      </c>
       <c r="C30" t="n">
         <v>448.9938888888888</v>
       </c>
@@ -81489,6 +81576,9 @@
         <is>
           <t>Run 30</t>
         </is>
+      </c>
+      <c r="B31" t="n">
+        <v>14.8115</v>
       </c>
       <c r="C31" t="n">
         <v>444.8438888888888</v>

</xml_diff>